<commit_message>
this is the first change
</commit_message>
<xml_diff>
--- a/FirstFile.xlsx
+++ b/FirstFile.xlsx
@@ -24,9 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>this is the first file added</t>
+  </si>
+  <si>
+    <t>first change</t>
   </si>
 </sst>
 </file>
@@ -344,10 +347,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -357,6 +360,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>